<commit_message>
1.5x consump for purines
</commit_message>
<xml_diff>
--- a/H1299_143B_prot-nucl-quant/asp_fate.xlsx
+++ b/H1299_143B_prot-nucl-quant/asp_fate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/lab-work/H1299_143B_prot-nucl-quant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AFF577-0983-3A4D-84AF-5A56A7122D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19546BD4-2C4D-9F4A-8A02-D99EAF2013AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2720" windowWidth="28800" windowHeight="13900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="133">
   <si>
     <t>H1299</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>Protein (Arg)</t>
+  </si>
+  <si>
+    <t>Efflux (Asn)*</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -628,14 +631,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3914,8 +3917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A47A286-DC8E-D14B-94A9-7E230954DBCC}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3929,16 +3932,16 @@
       <c r="B1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
       <c r="L1" s="16" t="s">
         <v>128</v>
       </c>
@@ -4209,15 +4212,15 @@
       <c r="F12" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="26">
         <f>G10/C10</f>
         <v>3.4909430261625164E-2</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="26">
         <f>H10/D10</f>
         <v>3.4902752520654952E-2</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="26">
         <f>I10/E10</f>
         <v>3.4908482741382467E-2</v>
       </c>
@@ -4263,8 +4266,8 @@
         <v>38.179456886414101</v>
       </c>
       <c r="G18" s="25">
-        <f>F18</f>
-        <v>38.179456886414101</v>
+        <f>F18*1.5</f>
+        <v>57.269185329621152</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
@@ -4273,24 +4276,24 @@
       </c>
       <c r="B19" s="25">
         <f>B18/(SUM($C$18:$G$18)-$E$18) *100</f>
-        <v>61.079631520784403</v>
+        <v>55.663519770034775</v>
       </c>
       <c r="C19" s="25">
         <f t="shared" ref="C19:G19" si="0">C18/(SUM($C$18:$G$18)-$E$18) *100</f>
-        <v>37.746776769582233</v>
+        <v>34.399658325603248</v>
       </c>
       <c r="D19" s="25">
         <f t="shared" si="0"/>
-        <v>23.332854751202177</v>
+        <v>21.263861444431527</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25">
         <f t="shared" si="0"/>
-        <v>19.460184239607802</v>
+        <v>17.734592091986098</v>
       </c>
       <c r="G19" s="25">
-        <f t="shared" si="0"/>
-        <v>19.460184239607802</v>
+        <f>G18/(SUM($C$18:$G$18)-$E$18) *100</f>
+        <v>26.601888137979145</v>
       </c>
       <c r="H19" s="25">
         <f>SUM(C19:G19)</f>
@@ -4303,31 +4306,31 @@
       </c>
       <c r="B20" s="25">
         <f>B18/(SUM($C$18:$G$18)) *100</f>
-        <v>45.203371648061093</v>
+        <v>42.166940328832659</v>
       </c>
       <c r="C20" s="25">
         <f t="shared" ref="C20:G20" si="1">C18/(SUM($C$18:$G$18)) *100</f>
-        <v>27.935361369218558</v>
+        <v>26.05886846431159</v>
       </c>
       <c r="D20" s="25">
         <f t="shared" si="1"/>
-        <v>17.268010278842542</v>
+        <v>16.108071864521069</v>
       </c>
       <c r="E20" s="25">
         <f t="shared" si="1"/>
-        <v>25.992723723817608</v>
+        <v>24.246722982953909</v>
       </c>
       <c r="F20" s="25">
         <f t="shared" si="1"/>
-        <v>14.401952314060647</v>
+        <v>13.434534675285379</v>
       </c>
       <c r="G20" s="25">
         <f t="shared" si="1"/>
-        <v>14.401952314060647</v>
+        <v>20.151802012928066</v>
       </c>
       <c r="H20" s="25">
         <f>SUM(C20:G20)</f>
-        <v>100.00000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
@@ -4478,33 +4481,33 @@
       <c r="A40" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="29">
+      <c r="B40" s="27">
         <f>M11</f>
         <v>4.1833284860424298</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40" s="27">
         <f>G10</f>
         <v>1.5980613096557379</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="27">
         <f>I10</f>
         <v>2.8811806680117367</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40" s="27">
         <f>B40-C40</f>
         <v>2.5852671763866919</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="27">
         <f>H10</f>
         <v>2.405026389683901</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="27">
         <f>N11</f>
         <v>1.3328230876029976</v>
       </c>
-      <c r="H40" s="29">
-        <f>N11</f>
-        <v>1.3328230876029976</v>
+      <c r="H40" s="27">
+        <f>N11*1.5</f>
+        <v>1.9992346314044964</v>
       </c>
       <c r="I40" s="25"/>
     </row>
@@ -4523,78 +4526,78 @@
       <c r="B44" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44" s="27">
         <f>D40</f>
         <v>2.8811806680117367</v>
       </c>
       <c r="D44" s="25">
         <f>C44/SUM($C$44:$C$49)*100</f>
-        <v>23.742377615276787</v>
+        <v>22.506422512238206</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B45" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45" s="27">
         <f>E40</f>
         <v>2.5852671763866919</v>
       </c>
       <c r="D45" s="25">
         <f t="shared" ref="D45:D49" si="2">C45/SUM($C$44:$C$49)*100</f>
-        <v>21.303901632975688</v>
+        <v>20.194886084298453</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B46" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="29">
+        <v>132</v>
+      </c>
+      <c r="C46" s="27">
         <f>F40</f>
         <v>2.405026389683901</v>
       </c>
       <c r="D46" s="25">
         <f t="shared" si="2"/>
-        <v>19.818626909636201</v>
+        <v>18.786930191594713</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B47" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="29">
+      <c r="C47" s="27">
         <f>C40</f>
         <v>1.5980613096557379</v>
       </c>
       <c r="D47" s="25">
         <f t="shared" si="2"/>
-        <v>13.16882883723963</v>
+        <v>12.483300139728085</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B48" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="29">
+      <c r="C48" s="27">
         <f>G40</f>
         <v>1.3328230876029976</v>
       </c>
       <c r="D48" s="25">
         <f t="shared" si="2"/>
-        <v>10.983132502435838</v>
+        <v>10.411384428856213</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="29">
+      <c r="C49" s="27">
         <f>H40</f>
-        <v>1.3328230876029976</v>
+        <v>1.9992346314044964</v>
       </c>
       <c r="D49" s="25">
         <f t="shared" si="2"/>
-        <v>10.983132502435838</v>
+        <v>15.617076643284319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>